<commit_message>
add mesh RE script
</commit_message>
<xml_diff>
--- a/devfile.xlsx
+++ b/devfile.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="91">
   <si>
     <t>DeviceID</t>
   </si>
@@ -34,13 +34,46 @@
     <t>Device-Type</t>
   </si>
   <si>
+    <t>QUwSDcl2ASZFQANSoKgOjUGUXQKpxwjzP1kVJAXhvzHLrhEPt6dw4C0Tha_3dm7W</t>
+  </si>
+  <si>
+    <t>z3UV9QwRYB0a-cW7zheCm5-w3OYecpCkiOOSvRPsjmXVVNlW8ieW2bbXAaj7v8on</t>
+  </si>
+  <si>
+    <t>-pSp3cJWLo5jIJucwoWgqYfFzu2tJQcXDruTMCfFZP3KbMObQdZQnnWwOwSiYuQA</t>
+  </si>
+  <si>
+    <t>u0XTyvoaV9Hz4_FLE3Rr8sqrJD6cDfbRFkX226tBpM-j0rS91yfPnmA_Volthc3v</t>
+  </si>
+  <si>
+    <t>j5zFq07CKJXQM80HePqC5RK80L-gh1rJh6IiMKGcClO-DfJVpEgMMLbKU0FXx7pu</t>
+  </si>
+  <si>
+    <t>CwkNE9l2s_NOUoUxYFLjai_bEQyJG1nZ0W-UgcBMKcEUrS3k3Ql7QwBvJnN1ugEs</t>
+  </si>
+  <si>
     <t>vZC-Qg9GyIDl32SE44YddRmAP6_nKg0Lf1O4Fh_Yo8Pzu-TUQrUAD4DhMOXTCbdB</t>
   </si>
   <si>
-    <t>j5zFq07CKJXQM80HePqC5RK80L-gh1rJh6IiMKGcClO-DfJVpEgMMLbKU0FXx7pu</t>
-  </si>
-  <si>
-    <t>C5P4qECsnb7vSydJBeg7btr5747VsESOdhg6YizgLB38lDfZ9lX9eJ2r_8i8mFBT</t>
+    <t>CjD6AafkLUhwoLzqgIW8JKgewZwGF6VI4bW2sI4A0qs7g1ZGuXO6rbbCNpel0f0S</t>
+  </si>
+  <si>
+    <t>piuNbmyRSm29ORfCSk9ROSQIb5CAJsh0pOdrcK4-wl0fllzE1ws4xBDNaSzeYoW0</t>
+  </si>
+  <si>
+    <t>h07Ab5DSHFbSpJMZhJA593mBbBUmw5Rl5Au_FWK4FsfzGWIQ2cFNXxNGI_2Fcmak</t>
+  </si>
+  <si>
+    <t>TbUKc1W_jAJfJC5Yb74-Edj2N_yRESFXKqcc0QQGHNko0nfzRdu5HjxiZe6Qz0Wd</t>
+  </si>
+  <si>
+    <t>TCD7FsU6vv5SwER9OVg3ZEg4PuuZVWRFpRgz5Wz6NL6X9H_q4Xx0RYO_2B3OnKUc</t>
+  </si>
+  <si>
+    <t>mPdUSXiIMTYJMIQJeJRCKZMsVwLz54pnMuCzZyfDpotOMkSamXnXR7IO1MdQ2WmX</t>
+  </si>
+  <si>
+    <t>9yzsY0Vi4oNGUEZNBRnwX3erSH5L9AllmNC_3MgxmSWQiloBzq8wANdrrjFcoNon</t>
   </si>
   <si>
     <t>JmcIw16f6q6eF_PMVmVk-WHN5DvNeKo4c3Fw0YKqBm6CqHqnXwYBBva3lSt8C-0y</t>
@@ -49,33 +82,6 @@
     <t>mn4qqGRXlEsgxVxPuZ-wFElcJiV0_wiHpkfrsWP1Mx-ccFel97uAbyBZuuPIEpI7</t>
   </si>
   <si>
-    <t>-pSp3cJWLo5jIJucwoWgqYfFzu2tJQcXDruTMCfFZP3KbMObQdZQnnWwOwSiYuQA</t>
-  </si>
-  <si>
-    <t>z3UV9QwRYB0a-cW7zheCm5-w3OYecpCkiOOSvRPsjmXVVNlW8ieW2bbXAaj7v8on</t>
-  </si>
-  <si>
-    <t>JmcIw16f6q6eF_PMVmVk-WHN5DvNeKo4c3Fw0YKqBm5wn2Lvy7RRNKFUYVEt_qLq</t>
-  </si>
-  <si>
-    <t>SlNmDWnymOUC_NdWairWfu0UeadTPSP3yx6WPcWFx3-1pbXZajP16Va9Izl-vFf3</t>
-  </si>
-  <si>
-    <t>9yzsY0Vi4oNGUEZNBRnwX3erSH5L9AllmNC_3MgxmSWQiloBzq8wANdrrjFcoNon</t>
-  </si>
-  <si>
-    <t>TbUKc1W_jAJfJC5Yb74-Edj2N_yRESFXKqcc0QQGHNko0nfzRdu5HjxiZe6Qz0Wd</t>
-  </si>
-  <si>
-    <t>mPdUSXiIMTYJMIQJeJRCKZMsVwLz54pnMuCzZyfDpotOMkSamXnXR7IO1MdQ2WmX</t>
-  </si>
-  <si>
-    <t>hAT_FYzKwhRH6DibgRqrsyizUTK3N3l0LCTx5INnu3Jln-ZgpM0s3fX1QzBFrxcL</t>
-  </si>
-  <si>
-    <t>mvECv-a_AhNfHlba5Q6_Ctp4oAfPMPrhvdY8lYnayIAKjjElc6q0DBUgMbgA3sp8</t>
-  </si>
-  <si>
     <t>K4ouszgY_l92YuT_5yqdOiHcZzfBFzmBZEtZFs5RXrI1dQsJnIJggleK38pHp_Z6</t>
   </si>
   <si>
@@ -85,16 +91,49 @@
     <t>oxn8uthuVz7ZhR1mI-dN0_DPoZd1hqNrZrJ1E3o5M3gSEsZTMWSXNxazgN7tkhoC</t>
   </si>
   <si>
-    <t>JmcIw16f6q6eF_PMVmVk-WHN5DvNeKo4c3Fw0YKqBm7ErqvCzuEGSVF1bM81JO3A</t>
+    <t>dL_Feznnvl_Eq6SiQ8nfkiujXj3GFfZGwmRxByPcUT6EOkxTqFW4T_J9rB6Si_bP</t>
+  </si>
+  <si>
+    <t>2219111B02429</t>
+  </si>
+  <si>
+    <t>2237193A00760</t>
+  </si>
+  <si>
+    <t>22221K3A00172</t>
+  </si>
+  <si>
+    <t>22465B9000110</t>
+  </si>
+  <si>
+    <t>2241584000038</t>
+  </si>
+  <si>
+    <t>2245034R00016</t>
   </si>
   <si>
     <t>2243627000112</t>
   </si>
   <si>
-    <t>2241584000038</t>
-  </si>
-  <si>
-    <t>2241078R00110</t>
+    <t>22482S0000148</t>
+  </si>
+  <si>
+    <t>22346B4000012</t>
+  </si>
+  <si>
+    <t>223A4B1000018</t>
+  </si>
+  <si>
+    <t>22360N3001322</t>
+  </si>
+  <si>
+    <t>22360N3001039</t>
+  </si>
+  <si>
+    <t>22431Q4000183</t>
+  </si>
+  <si>
+    <t>22360N3001370</t>
   </si>
   <si>
     <t>223CACS000016</t>
@@ -103,33 +142,6 @@
     <t>22334M3002425</t>
   </si>
   <si>
-    <t>22221K3A00172</t>
-  </si>
-  <si>
-    <t>2237193A00760</t>
-  </si>
-  <si>
-    <t>223CACS000007</t>
-  </si>
-  <si>
-    <t>2241542000128</t>
-  </si>
-  <si>
-    <t>22360N3001370</t>
-  </si>
-  <si>
-    <t>22360N3001322</t>
-  </si>
-  <si>
-    <t>22431Q4000183</t>
-  </si>
-  <si>
-    <t>22431Q4000377</t>
-  </si>
-  <si>
-    <t>2241542000280</t>
-  </si>
-  <si>
     <t>223A4B1000236</t>
   </si>
   <si>
@@ -139,16 +151,49 @@
     <t>2241584000037</t>
   </si>
   <si>
-    <t>223CACS000010</t>
+    <t>2241542000290</t>
+  </si>
+  <si>
+    <t>E4C32AD28FC4</t>
+  </si>
+  <si>
+    <t>5091E3E64470</t>
+  </si>
+  <si>
+    <t>54AF97557F2C</t>
+  </si>
+  <si>
+    <t>F0090D676B60</t>
+  </si>
+  <si>
+    <t>74FECEDAE1E2</t>
+  </si>
+  <si>
+    <t>6083E7C01398</t>
   </si>
   <si>
     <t>2023515A2B98</t>
   </si>
   <si>
-    <t>74FECEDAE1E2</t>
-  </si>
-  <si>
-    <t>74FECED2FEE8</t>
+    <t>7CF17E38C6EE</t>
+  </si>
+  <si>
+    <t>5C628BF46D0F</t>
+  </si>
+  <si>
+    <t>A842A1A4C394</t>
+  </si>
+  <si>
+    <t>40ED00CB1D2F</t>
+  </si>
+  <si>
+    <t>40ED00CB19DE</t>
+  </si>
+  <si>
+    <t>40AE30999B7A</t>
+  </si>
+  <si>
+    <t>40ED00CB1DBF</t>
   </si>
   <si>
     <t>20362690B8F5</t>
@@ -157,33 +202,6 @@
     <t>788CB5C7D660</t>
   </si>
   <si>
-    <t>54AF97557F2C</t>
-  </si>
-  <si>
-    <t>5091E3E64470</t>
-  </si>
-  <si>
-    <t>20362690B8DA</t>
-  </si>
-  <si>
-    <t>74FECECE52E5</t>
-  </si>
-  <si>
-    <t>40ED00CB1DBF</t>
-  </si>
-  <si>
-    <t>40ED00CB1D2F</t>
-  </si>
-  <si>
-    <t>40AE30999B7A</t>
-  </si>
-  <si>
-    <t>40AE30999DC0</t>
-  </si>
-  <si>
-    <t>74FECECE54AD</t>
-  </si>
-  <si>
     <t>A842A1A4CC18</t>
   </si>
   <si>
@@ -193,82 +211,82 @@
     <t>74FECEDAE1D8</t>
   </si>
   <si>
-    <t>20362690B8E3</t>
-  </si>
-  <si>
-    <t>0.1.0 3.0.0 v60be.0 Build 240507 Rel.64618n</t>
+    <t>74FECECE54CB</t>
+  </si>
+  <si>
+    <t>2.5.14 Build 20240827 Rel. 31177</t>
+  </si>
+  <si>
+    <t>2.0.0 Build 20220408 Rel. 70690</t>
+  </si>
+  <si>
+    <t>0.1.0 3.0.0 v60d5.0 Build 240918 Rel.44802n_Beta</t>
   </si>
   <si>
     <t>0.1.0 3.0.0 v60af.0 Build 240424 Rel.48510n</t>
   </si>
   <si>
+    <t>0.2.0 3.0.0 v60be.0 Build 240906 Rel.40026n</t>
+  </si>
+  <si>
+    <t>0.4.0 3.0.0 v6095.0 Build 240812 Rel.12929n</t>
+  </si>
+  <si>
     <t>0.3.0 3.0.0 v6095.0 Build 240509 Rel.21531n</t>
   </si>
   <si>
+    <t>0.16.0 2.0.0 v605f.0 Build 240430 Rel.29144n</t>
+  </si>
+  <si>
+    <t>0.9.0 3.0.0 v6065.0 Build 240806 Rel.46875n</t>
+  </si>
+  <si>
+    <t>0.17.0 2.0.0 v605f.0 Build 240522 Rel.4911n</t>
+  </si>
+  <si>
     <t>0.1.0 3.1.9 v60b3.0 Build 240515 Rel.78630n</t>
   </si>
   <si>
     <t>0.6.0 3.0.0 v6066.0 Build 220630 Rel.56119n</t>
   </si>
   <si>
-    <t>2.0.8 Build 20240524 Rel. 61926</t>
-  </si>
-  <si>
-    <t>2.0.6 Build 20230928 Rel. 882</t>
-  </si>
-  <si>
-    <t>0.3.0 3.1.7 v60b3.0 Build 240628 Rel.40574n</t>
-  </si>
-  <si>
-    <t>0.9.0 3.0.0 v6097.0 Build 240712 Rel.44731n_Beta</t>
-  </si>
-  <si>
-    <t>0.15.0 2.0.0 v605f.0 Build 240304 Rel.29932n</t>
-  </si>
-  <si>
-    <t>0.16.0 2.0.0 v605f.0 Build 240430 Rel.29144n</t>
-  </si>
-  <si>
-    <t>0.8.0 3.0.0 v6065.0 Build 240520 Rel.43161n</t>
-  </si>
-  <si>
-    <t>0.9.0 3.0.0 v6065.0 Build 240806 Rel.46875n</t>
-  </si>
-  <si>
-    <t>0.1.0 3.0.0 v60be.0 Build 240413 Rel.28782n_Beta</t>
+    <t>Deco M5</t>
+  </si>
+  <si>
+    <t>Deco X50</t>
+  </si>
+  <si>
+    <t>HB210 Pro</t>
+  </si>
+  <si>
+    <t>HB610V2</t>
   </si>
   <si>
     <t>HB710</t>
   </si>
   <si>
-    <t>HB610V2</t>
-  </si>
-  <si>
     <t>HB810</t>
   </si>
   <si>
+    <t>HX220</t>
+  </si>
+  <si>
+    <t>HX510</t>
+  </si>
+  <si>
     <t>EX921v</t>
   </si>
   <si>
     <t>XX230v</t>
   </si>
   <si>
-    <t>Deco X50</t>
-  </si>
-  <si>
     <t>HX510-PoE</t>
   </si>
   <si>
-    <t>HX220</t>
-  </si>
-  <si>
-    <t>HX510</t>
+    <t>DECO</t>
   </si>
   <si>
     <t>AGINET</t>
-  </si>
-  <si>
-    <t>DECO</t>
   </si>
 </sst>
 </file>
@@ -626,7 +644,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -660,19 +678,19 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D2" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="E2" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="F2" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="G2" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -683,19 +701,19 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D3" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="E3" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="F3" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="G3" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -706,19 +724,19 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D4" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="E4" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="F4" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="G4" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -729,19 +747,19 @@
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D5" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E5" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="F5" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="G5" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -752,19 +770,19 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D6" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="E6" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="F6" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="G6" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -775,19 +793,19 @@
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D7" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E7" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="F7" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="G7" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -798,19 +816,19 @@
         <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D8" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="E8" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="F8" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="G8" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -821,19 +839,19 @@
         <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D9" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E9" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="F9" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="G9" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -844,19 +862,19 @@
         <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D10" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="E10" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="F10" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="G10" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -867,19 +885,19 @@
         <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D11" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="E11" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="F11" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="G11" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -890,19 +908,19 @@
         <v>16</v>
       </c>
       <c r="C12" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D12" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="E12" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="F12" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="G12" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -913,19 +931,19 @@
         <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D13" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E13" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="F13" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G13" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -936,19 +954,19 @@
         <v>18</v>
       </c>
       <c r="C14" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D14" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="E14" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="F14" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="G14" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -959,19 +977,19 @@
         <v>19</v>
       </c>
       <c r="C15" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D15" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="E15" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="F15" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="G15" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -982,19 +1000,19 @@
         <v>20</v>
       </c>
       <c r="C16" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D16" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="E16" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="F16" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="G16" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -1005,19 +1023,19 @@
         <v>21</v>
       </c>
       <c r="C17" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D17" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="E17" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="F17" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
       <c r="G17" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -1028,19 +1046,19 @@
         <v>22</v>
       </c>
       <c r="C18" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D18" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="E18" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="F18" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="G18" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -1051,16 +1069,62 @@
         <v>23</v>
       </c>
       <c r="C19" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D19" t="s">
-        <v>59</v>
+        <v>63</v>
+      </c>
+      <c r="E19" t="s">
+        <v>70</v>
       </c>
       <c r="F19" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="G19" t="s">
-        <v>83</v>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="1">
+        <v>0</v>
+      </c>
+      <c r="B20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" t="s">
+        <v>44</v>
+      </c>
+      <c r="D20" t="s">
+        <v>64</v>
+      </c>
+      <c r="E20" t="s">
+        <v>69</v>
+      </c>
+      <c r="F20" t="s">
+        <v>81</v>
+      </c>
+      <c r="G20" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="1">
+        <v>0</v>
+      </c>
+      <c r="B21" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" t="s">
+        <v>45</v>
+      </c>
+      <c r="D21" t="s">
+        <v>65</v>
+      </c>
+      <c r="F21" t="s">
+        <v>88</v>
+      </c>
+      <c r="G21" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>